<commit_message>
Update expected transaction data in user_data Excel file for accuracy
</commit_message>
<xml_diff>
--- a/test_e2e/main-treasury-temp/user_data/data__expected_trn.xlsx
+++ b/test_e2e/main-treasury-temp/user_data/data__expected_trn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\EfPrivate\EfDev3.STEX\financialmodel.test\005\_startup.Tests.Assets\9a10-reports-loan-positive and negative, final zero value, expired [REL]\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\test_e2e\main-treasury-temp\user_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547B51FD-B96F-4ED6-8FB7-6E2A3B638610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF16B6E7-85F1-4FDB-AFAE-FA5FEDC3DB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,10 +428,10 @@
     <t>credito v/qualcuno</t>
   </si>
   <si>
-    <t>['2020-10-31', '2020-12-31', '2022-10-31', '2022-12-31']</t>
-  </si>
-  <si>
     <t>[20, -30, 30, -20]</t>
+  </si>
+  <si>
+    <t>["2020-10-31", "2020-12-31", "2022-10-31", "2022-12-31"]</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1291,10 +1291,10 @@
         <v>0</v>
       </c>
       <c r="U9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="V9" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">

</xml_diff>